<commit_message>
update 2024 normalo data
</commit_message>
<xml_diff>
--- a/data/normalo2024.xlsx
+++ b/data/normalo2024.xlsx
@@ -1,37 +1,115 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelhaas/Documents/Coding/aytogermany/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568C7F2D-AF2F-EC42-9D7A-997454B366CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="21180" yWindow="780" windowWidth="13020" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nights" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Nights" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>Sidar</t>
+  </si>
+  <si>
+    <t>Sandro</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Gerrit</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Paddy</t>
+  </si>
+  <si>
+    <t>Eti</t>
+  </si>
+  <si>
+    <t>Paulo</t>
+  </si>
+  <si>
+    <t>Lights</t>
+  </si>
+  <si>
+    <t>Lina</t>
+  </si>
+  <si>
+    <t>Sina</t>
+  </si>
+  <si>
+    <t>Tais</t>
+  </si>
+  <si>
+    <t>Jana</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Pia</t>
+  </si>
+  <si>
+    <t>Lisa-Marie</t>
+  </si>
+  <si>
+    <t>Shelly</t>
+  </si>
+  <si>
+    <t>Edda</t>
+  </si>
+  <si>
+    <t>Maja</t>
+  </si>
+  <si>
+    <t>Afra</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +124,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,74 +448,124 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="B1:L1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Wilson</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Sidar</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Sandro</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Ryan</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Martin</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Gerrit</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Kevin</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Paddy</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Eti</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Paulo</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Lights</t>
-        </is>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moving code, writing on new solution generator
</commit_message>
<xml_diff>
--- a/data/normalo2024.xlsx
+++ b/data/normalo2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelhaas/Documents/Coding/aytogermany/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568C7F2D-AF2F-EC42-9D7A-997454B366CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F3E7FC-E61D-7943-8E52-D9E4C478264E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21180" yWindow="780" windowWidth="13020" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18920" yWindow="780" windowWidth="15280" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nights" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Wilson</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Afra</t>
+  </si>
+  <si>
+    <t>Mela</t>
   </si>
 </sst>
 </file>
@@ -449,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -568,6 +571,44 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Data and code changes for episodes 9/10
</commit_message>
<xml_diff>
--- a/data/normalo2024.xlsx
+++ b/data/normalo2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelhaas/Documents/Coding/aytogermany/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F3E7FC-E61D-7943-8E52-D9E4C478264E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1933986-E2DD-8148-B992-6F5EDD373401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18920" yWindow="780" windowWidth="15280" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7780" yWindow="780" windowWidth="26420" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nights" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>Wilson</t>
   </si>
@@ -110,12 +110,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -145,11 +157,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -499,7 +513,7 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
@@ -508,13 +522,13 @@
       <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H2" t="s">
@@ -526,7 +540,7 @@
       <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L2">
@@ -537,7 +551,7 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C3" t="s">
@@ -552,13 +566,13 @@
       <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J3" t="s">
@@ -575,7 +589,7 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
@@ -590,10 +604,10 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I4" t="s">
@@ -607,6 +621,44 @@
       </c>
       <c r="L4">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data episode 11-14 + some small changes/additions
</commit_message>
<xml_diff>
--- a/data/normalo2024.xlsx
+++ b/data/normalo2024.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelhaas/Documents/Coding/aytogermany/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1933986-E2DD-8148-B992-6F5EDD373401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA541F91-CF39-1945-85A1-810DCF6B9968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="780" windowWidth="26420" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18640" yWindow="780" windowWidth="15280" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nights" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="23">
   <si>
     <t>Wilson</t>
   </si>
@@ -95,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,8 +110,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,6 +133,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -157,13 +176,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -516,28 +538,28 @@
       <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="3" t="s">
@@ -554,31 +576,31 @@
       <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L3">
@@ -595,7 +617,7 @@
       <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
@@ -610,7 +632,7 @@
       <c r="H4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J4" t="s">
@@ -630,38 +652,126 @@
       <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L5">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55B11DEB-4A4C-C747-BAAE-DAFEAF7FBB70}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
All data for normalo 2024
</commit_message>
<xml_diff>
--- a/data/normalo2024.xlsx
+++ b/data/normalo2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelhaas/Documents/Coding/aytogermany/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA541F91-CF39-1945-85A1-810DCF6B9968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE34A212-D816-3F4A-B0CE-63D43DA33530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18640" yWindow="780" windowWidth="15280" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="23">
   <si>
     <t>Wilson</t>
   </si>
@@ -144,7 +144,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -176,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -186,6 +186,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -535,7 +536,7 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -550,7 +551,7 @@
       <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -588,7 +589,7 @@
       <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="3" t="s">
@@ -597,7 +598,7 @@
       <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="4" t="s">
         <v>21</v>
       </c>
       <c r="K3" s="6" t="s">
@@ -611,7 +612,7 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
@@ -623,10 +624,10 @@
       <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -635,10 +636,10 @@
       <c r="I4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="L4">
@@ -664,7 +665,7 @@
       <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -673,7 +674,7 @@
       <c r="I5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="K5" s="6" t="s">
@@ -699,7 +700,7 @@
       <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -711,10 +712,10 @@
       <c r="I6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="L6">
@@ -728,28 +729,28 @@
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="I7" t="s">
         <v>19</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K7" s="4" t="s">
@@ -757,6 +758,158 @@
       </c>
       <c r="L7">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>